<commit_message>
updated template with corrections
</commit_message>
<xml_diff>
--- a/RCaN/CaN_input_template.xlsx
+++ b/RCaN/CaN_input_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="129">
   <si>
     <t xml:space="preserve">Template for input data to CaN models</t>
   </si>
@@ -143,6 +143,9 @@
     <t xml:space="preserve">To</t>
   </si>
   <si>
+    <t xml:space="preserve">Trophic</t>
+  </si>
+  <si>
     <t xml:space="preserve">F01</t>
   </si>
   <si>
@@ -272,16 +275,22 @@
     <t xml:space="preserve">Constraint</t>
   </si>
   <si>
+    <t xml:space="preserve">Time-range</t>
+  </si>
+  <si>
     <t xml:space="preserve">C01</t>
   </si>
   <si>
-    <t xml:space="preserve">F01+F02+F03&lt;=MaxPrimaryProduction * 0.65</t>
+    <t xml:space="preserve">F01+F02+F03&lt;=MaxPrimaryProduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1988:2013</t>
   </si>
   <si>
     <t xml:space="preserve">C02</t>
   </si>
   <si>
-    <t xml:space="preserve">-(F01+F02+F03)&lt;=-MinPrimaryProduction* 0.65</t>
+    <t xml:space="preserve">-(F01+F02+F03)&lt;=-MinPrimaryProduction</t>
   </si>
   <si>
     <t xml:space="preserve">C03</t>
@@ -483,11 +492,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -510,8 +519,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="243" zoomScaleNormal="243" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -613,13 +622,12 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,7 +659,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>24</v>
       </c>
@@ -659,18 +667,15 @@
         <v>25</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,7 +881,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>35</v>
       </c>
@@ -900,10 +905,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -921,10 +926,13 @@
       <c r="C1" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>24</v>
@@ -932,10 +940,14 @@
       <c r="C2" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>24</v>
@@ -943,10 +955,14 @@
       <c r="C3" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>24</v>
@@ -954,10 +970,14 @@
       <c r="C4" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>26</v>
@@ -965,10 +985,14 @@
       <c r="C5" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>26</v>
@@ -976,10 +1000,14 @@
       <c r="C6" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>27</v>
@@ -987,10 +1015,14 @@
       <c r="C7" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>27</v>
@@ -998,10 +1030,14 @@
       <c r="C8" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>29</v>
@@ -1009,10 +1045,14 @@
       <c r="C9" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>29</v>
@@ -1020,10 +1060,14 @@
       <c r="C10" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>29</v>
@@ -1031,10 +1075,14 @@
       <c r="C11" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>29</v>
@@ -1042,10 +1090,14 @@
       <c r="C12" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>29</v>
@@ -1053,10 +1105,14 @@
       <c r="C13" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>29</v>
@@ -1064,10 +1120,14 @@
       <c r="C14" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>30</v>
@@ -1075,10 +1135,14 @@
       <c r="C15" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>30</v>
@@ -1086,10 +1150,14 @@
       <c r="C16" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>31</v>
@@ -1097,10 +1165,14 @@
       <c r="C17" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>31</v>
@@ -1108,10 +1180,14 @@
       <c r="C18" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>31</v>
@@ -1119,10 +1195,14 @@
       <c r="C19" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>31</v>
@@ -1130,10 +1210,14 @@
       <c r="C20" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>31</v>
@@ -1141,10 +1225,14 @@
       <c r="C21" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>32</v>
@@ -1152,10 +1240,14 @@
       <c r="C22" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>32</v>
@@ -1163,10 +1255,14 @@
       <c r="C23" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>32</v>
@@ -1174,16 +1270,24 @@
       <c r="C24" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>35</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1204,7 +1308,7 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1226,57 +1330,57 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.49"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="J1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1976,7 +2080,7 @@
       <c r="L14" s="0" t="n">
         <v>8.5405</v>
       </c>
-      <c r="M14" s="1" t="n">
+      <c r="M14" s="2" t="n">
         <v>1050000</v>
       </c>
       <c r="N14" s="0" t="n">
@@ -2031,7 +2135,7 @@
       <c r="L15" s="0" t="n">
         <v>8.7324</v>
       </c>
-      <c r="M15" s="1" t="n">
+      <c r="M15" s="2" t="n">
         <v>1170000</v>
       </c>
       <c r="N15" s="0" t="n">
@@ -2086,7 +2190,7 @@
       <c r="L16" s="0" t="n">
         <v>8.10525</v>
       </c>
-      <c r="M16" s="1" t="n">
+      <c r="M16" s="2" t="n">
         <v>1110000</v>
       </c>
       <c r="N16" s="0" t="n">
@@ -2196,7 +2300,7 @@
       <c r="L18" s="0" t="n">
         <v>2.18995</v>
       </c>
-      <c r="M18" s="1" t="n">
+      <c r="M18" s="2" t="n">
         <v>1070000</v>
       </c>
       <c r="N18" s="0" t="n">
@@ -2306,7 +2410,7 @@
       <c r="L20" s="0" t="n">
         <v>5.14895</v>
       </c>
-      <c r="M20" s="1" t="n">
+      <c r="M20" s="2" t="n">
         <v>1100000</v>
       </c>
       <c r="N20" s="0" t="n">
@@ -2526,7 +2630,7 @@
       <c r="L24" s="0" t="n">
         <v>2.18225</v>
       </c>
-      <c r="M24" s="1" t="n">
+      <c r="M24" s="2" t="n">
         <v>1130000</v>
       </c>
       <c r="N24" s="0" t="n">
@@ -2581,7 +2685,7 @@
       <c r="L25" s="0" t="n">
         <v>2.625</v>
       </c>
-      <c r="M25" s="1" t="n">
+      <c r="M25" s="2" t="n">
         <v>1230000</v>
       </c>
       <c r="N25" s="0" t="n">
@@ -2636,7 +2740,7 @@
       <c r="L26" s="0" t="n">
         <v>2.25135</v>
       </c>
-      <c r="M26" s="1" t="n">
+      <c r="M26" s="2" t="n">
         <v>1110000</v>
       </c>
       <c r="N26" s="0" t="n">
@@ -2691,7 +2795,7 @@
       <c r="L27" s="0" t="n">
         <v>2.955</v>
       </c>
-      <c r="M27" s="1" t="n">
+      <c r="M27" s="2" t="n">
         <v>1190000</v>
       </c>
       <c r="N27" s="0" t="n">
@@ -2725,201 +2829,270 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="182" zoomScaleNormal="182" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>